<commit_message>
[feat] 1. tc 업데이트
</commit_message>
<xml_diff>
--- a/TC Directory/To Do List Test Case.xlsx
+++ b/TC Directory/To Do List Test Case.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhsdb\Desktop\포트폴리오\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B761D9-98C5-435D-8641-B08D22613FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD8BAD2-0BC0-46D1-9C33-CED5AC609920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6C457D58-EB79-43DF-AE70-B6D33573AE26}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6C457D58-EB79-43DF-AE70-B6D33573AE26}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Summary Report" sheetId="2" r:id="rId1"/>
+    <sheet name="To Do" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To Do'!$A$1:$K$87</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="309">
   <si>
     <t>Depth1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -448,14 +449,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>list</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>수정</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>To Do 수정</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -721,10 +714,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>삭제</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1. list 우측 삭제 버튼 클릭
 2. alert 의 확인버튼 클릭</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -775,10 +764,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>검색</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>TC ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -826,10 +811,6 @@
   </si>
   <si>
     <t>TC00000003</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>빈값으로 확인</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -999,10 +980,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>caret 표시는 나중에 다시 확인</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>OK</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1020,6 +997,356 @@
   </si>
   <si>
     <t>TC00000028</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 현재 화면 유지하며, alert 표시
+("내용 or 날짜를 입력하세요.", 확인버튼)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 신규 to do 생성(API)
+2. 사이트 접속
+3. list 존재</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>To Do 삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>To Do 검색</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 생성한 to do의 제목을 search bar의 좌측 입력란에 입력
+2. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 기존의 "내용을 입력하세요." text 사라지며 입력한 text 표시
+2. 검색 결과 입력한 text와 제목이 일치하는 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 생성한 to do 중 하나의 to do 제목을 search bar의 좌측 입력란에 입력
+2. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>제목 검색</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>미입력 시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 생성한 to do 중 하나의 to do 제목의 일부를 search bar의 좌측 입력란에 입력
+(ex. 생성 todo 제목 : test title / 입력할 제목 : test ti
+2. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 검색 결과 입력한 text와 제목이 일치하는 2개의 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 날짜와 제목이 다른 2개의 신규 to do 생성(API)
+2. 사이트 접속
+3. list 존재</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 날짜는 다르고, 제목이 같은 2개의 신규 to do 생성(API)
+2. 사이트 접속
+3. list 존재</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 생성한 to do 제목의 일부를 search bar의 좌측 입력란에 입력
+(ex. 생성 todo 제목 : test title / 입력할 제목 : test ti
+2. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 검색 결과 제목에 입력한 text가 포함된 2개의 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 검색 결과 제목에 입력한 text가 포함된 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 날짜는 같고, 제목이 다른 2개의 신규 to do 생성(API)
+2. 사이트 접속
+3. list 존재</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 검색 결과 입력한 text와 제목이 일치하는 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 날짜와 제목이 같은 2개의 신규 to do 생성(API)
+2. 사이트 접속
+3. list 존재</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>날짜 검색</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 생성한 to do 중 하나의 to do 날짜를 search bar의 우측 날짜란에 입력
+2. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 기존의 "연도-월-일" 에서 입력한 날짜로 변경되어 표시
+2. 검색 결과 입력한 날짜와 일치하는 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 검색 결과 입력한 날짜와 일치하는 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 생성한 to do의 날짜를 search bar의 우측 날짜란에 입력
+2. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 검색 결과 입력한 날짜와 일치하는 2개의 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 생성한 to do와 전혀 다른 제목을 search bar의 좌측 입력란에 입력
+2. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 검색 결과 아무것도 표시하지 않음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 생성한 to do와 전혀 다른 날짜를 search bar의 우측 날짜란에 입력
+2. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>제목+날짜 검색</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 생성한 to do와 전혀 다른 제목과 날짜를 search bar에 입력
+2. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 생성한 to do 중 하나의 to do 제목, 날짜를 search bar에 입력
+2. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 기존의 "내용을 입력하세요.", "연도-월-일" 에서 입력한 제목과 날짜로 변경되어 표시
+2. 검색 결과 입력한 제목, 날짜와 일치하는 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 생성한 to do 중 하나의 to do 제목의 일부, 날짜를 search bar에 입력
+(ex. 생성 todo 제목 : test title / 입력할 제목 : test ti
+2. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 검색 결과 날짜가 일치하며, 제목에 입력한 text가 포함된 to do list 표시</t>
+  </si>
+  <si>
+    <t>2. 검색 결과 날짜가 일치하며, 제목에 입력한 text가 포함된 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 검색 결과 입력한 제목, 날짜와 일치하는 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 생성한 to do의 제목, 날짜를 search bar에 입력
+2. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 검색 결과 입력한 제목, 날짜와 일치하는 2개의 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 생성한 to do의 제목의 일부, 날짜를 search bar에 입력
+(ex. 생성 todo 제목 : test title / 입력할 제목 : test ti
+2. 검색 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 검색 결과 날짜가 일치하며, 제목에 입력한 text가 포함된 2개의 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 검색 결과 입력한 제목, 날짜와 일치하는 to do list
+표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>List 스크롤</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 8개 이상의 to do 생성(API)
+2. 사이트 접속
+3. 8개 이상의 list 존재
+4. list 스크롤바 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 스크롤바 동작 확인</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 스크롤바 움직임에 따라 화면 정상 동작</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동화 테스트</t>
+  </si>
+  <si>
+    <t>자동화 테스트</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동화 테스트
+(빈값으로 확인)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동화 테스트
+(caret 표시는 나중에 다시 확인)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC00000061</t>
+  </si>
+  <si>
+    <t>TC00000062</t>
+  </si>
+  <si>
+    <t>TC00000063</t>
+  </si>
+  <si>
+    <t>TC00000064</t>
+  </si>
+  <si>
+    <t>TC00000065</t>
+  </si>
+  <si>
+    <t>TC00000066</t>
+  </si>
+  <si>
+    <t>TC00000067</t>
+  </si>
+  <si>
+    <t>TC00000068</t>
+  </si>
+  <si>
+    <t>TC00000069</t>
+  </si>
+  <si>
+    <t>TC00000070</t>
+  </si>
+  <si>
+    <t>TC00000071</t>
+  </si>
+  <si>
+    <t>TC00000072</t>
+  </si>
+  <si>
+    <t>TC00000073</t>
+  </si>
+  <si>
+    <t>TC00000074</t>
+  </si>
+  <si>
+    <t>TC00000075</t>
+  </si>
+  <si>
+    <t>TC00000076</t>
+  </si>
+  <si>
+    <t>TC00000077</t>
+  </si>
+  <si>
+    <t>TC00000078</t>
+  </si>
+  <si>
+    <t>TC00000079</t>
+  </si>
+  <si>
+    <t>TC00000080</t>
+  </si>
+  <si>
+    <t>TC00000081</t>
+  </si>
+  <si>
+    <t>TC00000082</t>
+  </si>
+  <si>
+    <t>TC00000083</t>
+  </si>
+  <si>
+    <t>TC00000084</t>
+  </si>
+  <si>
+    <t>TC00000085</t>
+  </si>
+  <si>
+    <t>To Do List</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 이름</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>버전</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>시작일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마감일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.02.08</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>박온유</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트 환경</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1027,7 +1354,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1052,6 +1379,14 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="72"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1068,12 +1403,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1128,19 +1463,6 @@
         <color theme="4" tint="-0.499984740745262"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color theme="4" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="-0.499984740745262"/>
-      </top>
       <bottom style="thin">
         <color theme="4" tint="-0.499984740745262"/>
       </bottom>
@@ -1256,13 +1578,145 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1290,16 +1744,10 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1326,7 +1774,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1341,20 +1789,239 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1367,6 +2034,75 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>583229</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>56614</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C5D5A30-DFEE-47B0-92AF-1649B9AB11F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3057525" y="1885950"/>
+          <a:ext cx="5383829" cy="2571214"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{1890FB2D-3CB3-4192-9AAE-F7798222C28A}" name="표11" displayName="표11" ref="B9:C12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <tableColumns count="2">
+    <tableColumn id="2" xr3:uid="{21F14843-527F-4754-A9C1-0296505EE905}" name="열2" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{FC00FDDE-C634-48AA-91EF-E45F10C3CA8C}" name="열3" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{AEA86320-2470-4054-B47D-92D8A347FEA2}" name="표11_141617" displayName="표11_141617" ref="N9:O10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <tableColumns count="2">
+    <tableColumn id="2" xr3:uid="{F91CD0AC-3E44-4937-BBC9-DF87733B1E4C}" name="열2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{7FBDD4C4-CBCB-49F5-AAD8-9DE506A2802D}" name="열3" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1665,11 +2401,228 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9314B11-EF42-4D25-8E4C-42205CF3F3B0}">
+  <dimension ref="A1:P12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.625" customWidth="1"/>
+    <col min="2" max="3" width="13.625" customWidth="1"/>
+    <col min="8" max="9" width="13.625" customWidth="1"/>
+    <col min="14" max="15" width="13.625" customWidth="1"/>
+    <col min="16" max="16" width="3.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="35" t="s">
+        <v>301</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="N9" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="O9" s="36" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="37" t="s">
+        <v>302</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>300</v>
+      </c>
+      <c r="N10" s="37" t="s">
+        <v>308</v>
+      </c>
+      <c r="O10" s="38"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="37" t="s">
+        <v>303</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="C12" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:P8"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77A7E11-AD39-4C68-8EFB-0359E0A3990C}">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1682,7 +2635,7 @@
     <col min="6" max="6" width="30.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="44.625" style="1" customWidth="1"/>
     <col min="8" max="8" width="45.25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="15.125" style="9" customWidth="1"/>
     <col min="10" max="10" width="10.625" style="1" customWidth="1"/>
     <col min="11" max="11" width="33.125" style="1" customWidth="1"/>
   </cols>
@@ -1701,7 +2654,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>14</v>
@@ -1723,10 +2676,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1734,7 +2687,7 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>10</v>
@@ -1745,21 +2698,23 @@
       <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>167</v>
+      <c r="I2" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>10</v>
@@ -1770,19 +2725,19 @@
       <c r="H3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="9"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>10</v>
@@ -1793,21 +2748,23 @@
       <c r="H4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>167</v>
+      <c r="I4" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
+      <c r="K4" s="19" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>10</v>
@@ -1818,23 +2775,23 @@
       <c r="H5" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>167</v>
+      <c r="I5" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
-        <v>172</v>
+      <c r="K5" s="7" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>10</v>
@@ -1845,21 +2802,23 @@
       <c r="H6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>167</v>
+      <c r="I6" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="K6" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>10</v>
@@ -1870,21 +2829,23 @@
       <c r="H7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>167</v>
+      <c r="I7" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25" t="s">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="6" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>81</v>
@@ -1895,19 +2856,21 @@
       <c r="H8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>167</v>
+      <c r="I8" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>45</v>
@@ -1916,23 +2879,25 @@
         <v>25</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>167</v>
+        <v>169</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>47</v>
@@ -1943,17 +2908,17 @@
       <c r="H10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="9"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>49</v>
@@ -1964,17 +2929,17 @@
       <c r="H11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="9"/>
+      <c r="I11" s="24"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>46</v>
@@ -1985,19 +2950,19 @@
       <c r="H12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="9"/>
+      <c r="I12" s="24"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>45</v>
@@ -2008,21 +2973,23 @@
       <c r="H13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>167</v>
+      <c r="I13" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+      <c r="K13" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>26</v>
@@ -2033,19 +3000,19 @@
       <c r="H14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>26</v>
@@ -2056,19 +3023,19 @@
       <c r="H15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23" t="s">
         <v>40</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>51</v>
@@ -2079,17 +3046,17 @@
       <c r="H16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="9"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>52</v>
@@ -2100,25 +3067,23 @@
       <c r="H17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="9"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="11" t="s">
+      <c r="B18" s="28" t="s">
         <v>87</v>
       </c>
+      <c r="C18" s="10"/>
       <c r="D18" s="3" t="s">
         <v>63</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>58</v>
@@ -2129,21 +3094,23 @@
       <c r="H18" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>167</v>
+      <c r="I18" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
+      <c r="K18" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="3"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>60</v>
@@ -2154,23 +3121,23 @@
       <c r="H19" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>167</v>
+      <c r="I19" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="7" t="s">
-        <v>224</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="11"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>60</v>
@@ -2181,23 +3148,23 @@
       <c r="H20" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I20" s="9" t="s">
-        <v>225</v>
+      <c r="I20" s="24" t="s">
+        <v>219</v>
       </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="3" t="s">
-        <v>224</v>
+      <c r="K20" s="7" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="14" t="s">
+      <c r="A21" s="21"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="11" t="s">
         <v>66</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>60</v>
@@ -2208,23 +3175,23 @@
       <c r="H21" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="I21" s="26" t="s">
-        <v>181</v>
+      <c r="I21" s="24" t="s">
+        <v>176</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="7" t="s">
-        <v>222</v>
+      <c r="A22" s="21"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="25" t="s">
+        <v>217</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>71</v>
@@ -2235,19 +3202,21 @@
       <c r="H22" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>167</v>
+      <c r="I22" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
+      <c r="K22" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="23" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="6"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="26"/>
       <c r="E23" s="6" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>71</v>
@@ -2258,19 +3227,21 @@
       <c r="H23" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>225</v>
+      <c r="I23" s="24" t="s">
+        <v>219</v>
       </c>
       <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
+      <c r="K23" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="6"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="26"/>
       <c r="E24" s="6" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>71</v>
@@ -2281,21 +3252,21 @@
       <c r="H24" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="I24" s="26" t="s">
-        <v>228</v>
+      <c r="I24" s="24" t="s">
+        <v>222</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="6"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="26"/>
       <c r="E25" s="6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>71</v>
@@ -2306,19 +3277,19 @@
       <c r="H25" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>225</v>
+      <c r="I25" s="24" t="s">
+        <v>219</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="6"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="26"/>
       <c r="E26" s="6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>73</v>
@@ -2329,21 +3300,21 @@
       <c r="H26" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I26" s="26" t="s">
-        <v>228</v>
+      <c r="I26" s="24" t="s">
+        <v>222</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="6"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="26"/>
       <c r="E27" s="6" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>73</v>
@@ -2354,19 +3325,21 @@
       <c r="H27" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>225</v>
+      <c r="I27" s="24" t="s">
+        <v>219</v>
       </c>
       <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
+      <c r="K27" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="23"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="6"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="6" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>77</v>
@@ -2377,21 +3350,21 @@
       <c r="H28" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="I28" s="26" t="s">
-        <v>228</v>
+      <c r="I28" s="24" t="s">
+        <v>222</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="24"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="6"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="27"/>
       <c r="E29" s="6" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>88</v>
@@ -2402,989 +3375,1348 @@
       <c r="H29" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I29" s="26" t="s">
-        <v>228</v>
+      <c r="I29" s="24" t="s">
+        <v>222</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="A30" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="B30" s="3"/>
+      <c r="C30" s="31" t="s">
         <v>92</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="6" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>47</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>225</v>
+        <v>95</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>219</v>
       </c>
       <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
+      <c r="K30" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="21"/>
       <c r="D31" s="3"/>
       <c r="E31" s="6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>47</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>225</v>
+        <v>97</v>
+      </c>
+      <c r="I31" s="24" t="s">
+        <v>219</v>
       </c>
       <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
+      <c r="K31" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="21"/>
       <c r="D32" s="3"/>
       <c r="E32" s="6" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>225</v>
+      <c r="I32" s="24" t="s">
+        <v>219</v>
       </c>
       <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
+      <c r="K32" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="33" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="C33" s="21"/>
       <c r="D33" s="3"/>
       <c r="E33" s="6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>225</v>
+        <v>103</v>
+      </c>
+      <c r="I33" s="24" t="s">
+        <v>219</v>
       </c>
       <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
+      <c r="K33" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="34" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="C34" s="21"/>
       <c r="D34" s="3"/>
       <c r="E34" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F34" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>225</v>
+      <c r="I34" s="24" t="s">
+        <v>219</v>
       </c>
       <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
+      <c r="K34" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="35" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="3"/>
       <c r="E35" s="6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>225</v>
+        <v>108</v>
+      </c>
+      <c r="I35" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
+      <c r="K35" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="36" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>225</v>
+        <v>115</v>
+      </c>
+      <c r="I36" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
+      <c r="K36" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="37" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="I37" s="26" t="s">
-        <v>228</v>
+        <v>114</v>
+      </c>
+      <c r="I37" s="24" t="s">
+        <v>176</v>
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
+      <c r="A38" s="21"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G38" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H38" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="H38" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I38" s="9"/>
+      <c r="I38" s="24"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
     </row>
     <row r="39" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I39" s="9"/>
+        <v>121</v>
+      </c>
+      <c r="I39" s="24"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
     </row>
     <row r="40" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A40" s="3"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="I40" s="9"/>
+        <v>117</v>
+      </c>
+      <c r="I40" s="24"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
     </row>
     <row r="41" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="I41" s="9"/>
+        <v>119</v>
+      </c>
+      <c r="I41" s="24"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
     </row>
     <row r="42" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="3"/>
+      <c r="A42" s="21"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G42" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H42" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="H42" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="I42" s="9"/>
+      <c r="I42" s="24"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
     </row>
     <row r="43" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A43" s="3"/>
+      <c r="A43" s="21"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="I43" s="9"/>
+        <v>115</v>
+      </c>
+      <c r="I43" s="24"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
     </row>
     <row r="44" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="I44" s="9"/>
+        <v>114</v>
+      </c>
+      <c r="I44" s="24"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
     </row>
     <row r="45" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A45" s="3"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G45" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H45" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="H45" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I45" s="9"/>
+      <c r="I45" s="24"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
     </row>
     <row r="46" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A46" s="3"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I46" s="9"/>
+        <v>121</v>
+      </c>
+      <c r="I46" s="24"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
     </row>
     <row r="47" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A47" s="3"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="I47" s="9"/>
+        <v>117</v>
+      </c>
+      <c r="I47" s="24"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
     </row>
     <row r="48" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A48" s="3"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="I48" s="9"/>
+        <v>119</v>
+      </c>
+      <c r="I48" s="24"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
     </row>
     <row r="49" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="3"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G49" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H49" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="H49" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="I49" s="9"/>
+      <c r="I49" s="24"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
     </row>
     <row r="50" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A50" s="3"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="I50" s="9"/>
+        <v>115</v>
+      </c>
+      <c r="I50" s="24"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
     </row>
     <row r="51" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A51" s="3"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="I51" s="9"/>
+        <v>114</v>
+      </c>
+      <c r="I51" s="24"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
     </row>
     <row r="52" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A52" s="3"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G52" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H52" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="H52" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I52" s="9"/>
+      <c r="I52" s="24"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
     </row>
     <row r="53" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A53" s="3"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I53" s="9"/>
+        <v>121</v>
+      </c>
+      <c r="I53" s="24"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
     </row>
     <row r="54" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A54" s="3"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="I54" s="9"/>
+        <v>117</v>
+      </c>
+      <c r="I54" s="24"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
     </row>
     <row r="55" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A55" s="3"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="I55" s="9"/>
+        <v>119</v>
+      </c>
+      <c r="I55" s="24"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
     </row>
     <row r="56" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A56" s="3"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G56" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H56" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="H56" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="I56" s="9"/>
+      <c r="I56" s="24"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
     </row>
     <row r="57" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A57" s="3"/>
+      <c r="A57" s="20" t="s">
+        <v>226</v>
+      </c>
       <c r="B57" s="3"/>
-      <c r="C57" s="3" t="s">
-        <v>146</v>
-      </c>
+      <c r="C57" s="3"/>
       <c r="D57" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="I57" s="9"/>
+        <v>145</v>
+      </c>
+      <c r="I57" s="24"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
     </row>
     <row r="58" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A58" s="3"/>
+      <c r="A58" s="21"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I58" s="9"/>
+        <v>147</v>
+      </c>
+      <c r="I58" s="24"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
     </row>
     <row r="59" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A59" s="3"/>
+      <c r="A59" s="21"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="I59" s="9"/>
+        <v>145</v>
+      </c>
+      <c r="I59" s="24"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
     </row>
     <row r="60" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A60" s="3"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I60" s="9"/>
+        <v>147</v>
+      </c>
+      <c r="I60" s="24"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
     </row>
     <row r="61" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A61" s="3"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="I61" s="9"/>
+        <v>145</v>
+      </c>
+      <c r="I61" s="24"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
     </row>
     <row r="62" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A62" s="3"/>
+      <c r="A62" s="22"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I62" s="9"/>
+        <v>147</v>
+      </c>
+      <c r="I62" s="24"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A63" s="3"/>
+    <row r="63" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A63" s="20" t="s">
+        <v>227</v>
+      </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="9"/>
+      <c r="D63" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="I63" s="24"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="9"/>
-      <c r="J64" s="3"/>
-      <c r="K64" s="3"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A65" s="3"/>
+    <row r="64" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A64" s="21"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="I64" s="24"/>
+      <c r="J64" s="19"/>
+      <c r="K64" s="19"/>
+    </row>
+    <row r="65" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A65" s="21"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="9"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="I65" s="24"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A66" s="3"/>
+    <row r="66" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A66" s="21"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="9"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="I66" s="24"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A67" s="3"/>
+    <row r="67" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A67" s="21"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="9"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="I67" s="24"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A68" s="3"/>
+    <row r="68" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A68" s="21"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="9"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="I68" s="24"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A69" s="3"/>
+    <row r="69" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A69" s="21"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-      <c r="I69" s="9"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="I69" s="24"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A70" s="3"/>
+    <row r="70" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A70" s="21"/>
       <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="9"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="I70" s="24"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A71" s="3"/>
+    <row r="71" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A71" s="21"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="9"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="I71" s="24"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" s="3"/>
+    <row r="72" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A72" s="21"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="9"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="I72" s="24"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="9"/>
-      <c r="J73" s="3"/>
-      <c r="K73" s="3"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A74" s="3"/>
+    <row r="73" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A73" s="21"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="I73" s="24"/>
+      <c r="J73" s="19"/>
+      <c r="K73" s="19"/>
+    </row>
+    <row r="74" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A74" s="21"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="9"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="I74" s="24"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A75" s="3"/>
+    <row r="75" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A75" s="21"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="4"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
-      <c r="I75" s="9"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="I75" s="24"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A76" s="3"/>
+    <row r="76" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A76" s="21"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
-      <c r="H76" s="4"/>
-      <c r="I76" s="9"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="I76" s="24"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="3"/>
+    <row r="77" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A77" s="21"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="9"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="I77" s="24"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
     </row>
+    <row r="78" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A78" s="21"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="E78" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="I78" s="24"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+    </row>
+    <row r="79" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A79" s="21"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="I79" s="24"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+    </row>
+    <row r="80" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A80" s="21"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="I80" s="24"/>
+      <c r="J80" s="19"/>
+      <c r="K80" s="19"/>
+    </row>
+    <row r="81" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A81" s="21"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="H81" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="I81" s="24"/>
+      <c r="J81" s="19"/>
+      <c r="K81" s="19"/>
+    </row>
+    <row r="82" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A82" s="21"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="I82" s="24"/>
+      <c r="J82" s="19"/>
+      <c r="K82" s="19"/>
+    </row>
+    <row r="83" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A83" s="21"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I83" s="24"/>
+      <c r="J83" s="19"/>
+      <c r="K83" s="19"/>
+    </row>
+    <row r="84" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A84" s="21"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="H84" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="I84" s="24"/>
+      <c r="J84" s="19"/>
+      <c r="K84" s="19"/>
+    </row>
+    <row r="85" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A85" s="21"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="I85" s="24"/>
+      <c r="J85" s="19"/>
+      <c r="K85" s="19"/>
+    </row>
+    <row r="86" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A86" s="22"/>
+      <c r="B86" s="19"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="H86" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="I86" s="24"/>
+      <c r="J86" s="19"/>
+      <c r="K86" s="19"/>
+    </row>
+    <row r="87" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A87" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B87" s="19"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="I87" s="24"/>
+      <c r="J87" s="19"/>
+      <c r="K87" s="19"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K77" xr:uid="{E77A7E11-AD39-4C68-8EFB-0359E0A3990C}"/>
-  <mergeCells count="7">
+  <autoFilter ref="A1:K87" xr:uid="{E77A7E11-AD39-4C68-8EFB-0359E0A3990C}"/>
+  <mergeCells count="16">
+    <mergeCell ref="C30:C35"/>
+    <mergeCell ref="A30:A56"/>
+    <mergeCell ref="A57:A62"/>
+    <mergeCell ref="A63:A86"/>
+    <mergeCell ref="D64:D72"/>
+    <mergeCell ref="D73:D77"/>
+    <mergeCell ref="D78:D86"/>
     <mergeCell ref="A18:A29"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="C8:C17"/>
@@ -3392,8 +4724,15 @@
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="C3:C6"/>
     <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D22:D29"/>
+    <mergeCell ref="B18:B29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(EXACT($I1, "NG"), LEN($I1)=2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[update] 1. StatusTest 수정 2. TC 수정
</commit_message>
<xml_diff>
--- a/TC Directory/To Do List Test Case.xlsx
+++ b/TC Directory/To Do List Test Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhsdb\Desktop\포트폴리오\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD8BAD2-0BC0-46D1-9C33-CED5AC609920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721D8355-61DA-4863-BE9B-8AB5664D46D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6C457D58-EB79-43DF-AE70-B6D33573AE26}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="318">
   <si>
     <t>Depth1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -565,23 +565,12 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1. to do 생성시에 입력한 제목, 내용, 날짜 표시
-2. list에 수정한 text로 제목 변경되어 표시
-3. 제목란에 변경된 제목으로 표시, 내용과 날짜는 변동 없음</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1. list 우측 수정 버튼 클릭
 2. 제목란과 내용란의 text를 임의로 수정 후 저장 클릭
 3. list 우측 수정 버튼 클릭</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>2. list에 수정한 text로 제목 변경되어 표시
-3. 제목과 내용이 변경된 내용으로 표시, 날짜는 변동 없음</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1. list 우측 수정 버튼 클릭
 2. 날짜와 내용 정보를 임의로 수정 후 저장 클릭
 3. list 우측 수정 버튼 클릭</t>
@@ -719,23 +708,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1. alert 표시
-("삭제하시겠습니까?", 확인버튼, 취소버튼)
-2. 해당 to do가 삭제되어 list에 표시되지 않음</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1. list 우측 삭제 버튼 클릭
 2. alert 의 취소버튼 클릭</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1. alert 표시
-("삭제하시겠습니까?", 확인버튼, 취소버튼)
-2. alert 사라지며 해당 to do 삭제되지 않고 유지</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>대기중
 -삭제 확인</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -845,14 +822,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>NG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>날짜를 선택할 수가 없음</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>TC00000022</t>
   </si>
   <si>
@@ -988,20 +957,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>날짜를 선택할 수가 없음</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>TC00000028</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 현재 화면 유지하며, alert 표시
-("내용 or 날짜를 입력하세요.", 확인버튼)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1021,10 +977,6 @@
   <si>
     <t>1. 생성한 to do의 제목을 search bar의 좌측 입력란에 입력
 2. 검색 버튼 클릭</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 검색 버튼 클릭</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1347,6 +1299,105 @@
   </si>
   <si>
     <t>테스트 환경</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동화 테스트
+(20240217)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동화 테스트
+(20240212)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동화 테스트
+(20240211)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HLD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HLD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동화 테스트시 날짜 선택 불가능으로 
+자동화 테스트 보류</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동화 테스트시 날짜 선택 불가능으로 
+자동화 테스트 보류</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 내용 수정 후 저장 시 진행 상태가 "대기중"으로 변경됨
+자동화 테스트
+(20240217)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. list에 수정한 text로 제목 변경되어 표시, 진행상태는 그대로 표시
+3. 제목과 내용이 변경된 내용으로 표시, 날짜는 변동 없음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. to do 생성시에 입력한 제목, 내용, 날짜 표시
+2. list에 수정한 text로 제목 변경되어 표시, 진행상태는 그대로 표시
+3. 제목란에 변경된 제목으로 표시, 내용과 날짜는 변동 없음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 제목 수정 후 저장 시 진행 상태가 "대기중"으로 변경됨
+자동화 테스트
+(20240217)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 제목, 내용 수정 후 저장 시 진행 상태가 "대기중"으로 변경됨
+자동화 테스트
+(20240217)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 검색 버튼 클릭
+2. 확인 버튼 클릭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 현재 화면 유지하며, alert 표시
+("내용 or 날짜를 입력하세요.", 확인버튼)
+2. alert 사라지며 화면 유지됨</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. confirm 표시
+("삭제하시겠습니까?", 확인버튼, 취소버튼)
+2. 해당 to do가 삭제되어 list에 표시되지 않음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. confirm 표시
+("삭제하시겠습니까?", 확인버튼, 취소버튼)
+2. alert 사라지며 해당 to do 삭제되지 않고 유지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. alert 미표시
+자동화 테스트
+(20240217)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1777,6 +1828,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1787,9 +1865,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1813,35 +1888,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1937,6 +1995,75 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2021,6 +2148,24 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -2041,15 +2186,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>583229</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>56614</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>8692</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2072,8 +2217,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3057525" y="1885950"/>
-          <a:ext cx="5383829" cy="2571214"/>
+          <a:off x="3048000" y="1695450"/>
+          <a:ext cx="5504617" cy="2628900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2086,20 +2231,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{1890FB2D-3CB3-4192-9AAE-F7798222C28A}" name="표11" displayName="표11" ref="B9:C12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{1890FB2D-3CB3-4192-9AAE-F7798222C28A}" name="표11" displayName="표11" ref="B9:C12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <tableColumns count="2">
-    <tableColumn id="2" xr3:uid="{21F14843-527F-4754-A9C1-0296505EE905}" name="열2" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{FC00FDDE-C634-48AA-91EF-E45F10C3CA8C}" name="열3" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{21F14843-527F-4754-A9C1-0296505EE905}" name="열2" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{FC00FDDE-C634-48AA-91EF-E45F10C3CA8C}" name="열3" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{AEA86320-2470-4054-B47D-92D8A347FEA2}" name="표11_141617" displayName="표11_141617" ref="N9:O10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{AEA86320-2470-4054-B47D-92D8A347FEA2}" name="표11_141617" displayName="표11_141617" ref="N9:O10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <tableColumns count="2">
-    <tableColumn id="2" xr3:uid="{F91CD0AC-3E44-4937-BBC9-DF87733B1E4C}" name="열2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{7FBDD4C4-CBCB-49F5-AAD8-9DE506A2802D}" name="열3" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{F91CD0AC-3E44-4937-BBC9-DF87733B1E4C}" name="열2" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{7FBDD4C4-CBCB-49F5-AAD8-9DE506A2802D}" name="열3" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DB75ED6-6D90-46D7-B8B2-4533B0C33786}" name="표11_2" displayName="표11_2" ref="B23:C33" headerRowCount="0" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <tableColumns count="2">
+    <tableColumn id="2" xr3:uid="{A747249A-E21E-43B1-AD54-F8DB00EAC198}" name="열2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{D99E7FC2-6B43-412B-96E6-1FCA5520DA32}" name="열3" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2402,10 +2557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9314B11-EF42-4D25-8E4C-42205CF3F3B0}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2418,190 +2573,234 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
-        <v>299</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
+      <c r="A1" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="35" t="s">
-        <v>301</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>299</v>
-      </c>
-      <c r="N9" s="35" t="s">
-        <v>306</v>
-      </c>
-      <c r="O9" s="36" t="s">
-        <v>307</v>
+      <c r="B9" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>289</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="O9" s="23" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="37" t="s">
-        <v>302</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>300</v>
-      </c>
-      <c r="N10" s="37" t="s">
-        <v>308</v>
-      </c>
-      <c r="O10" s="38"/>
+      <c r="B10" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="N10" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="O10" s="25"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="37" t="s">
-        <v>303</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>305</v>
+      <c r="B11" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="34" t="s">
-        <v>304</v>
-      </c>
-      <c r="C12" s="39"/>
+      <c r="B12" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="C12" s="26"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="24"/>
+      <c r="C25" s="25"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="21"/>
+      <c r="C26" s="26"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="24"/>
+      <c r="C27" s="25"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="24"/>
+      <c r="C28" s="25"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="21"/>
+      <c r="C33" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2610,9 +2809,10 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2621,8 +2821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77A7E11-AD39-4C68-8EFB-0359E0A3990C}">
   <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2637,7 +2837,7 @@
     <col min="8" max="8" width="45.25" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.125" style="9" customWidth="1"/>
     <col min="10" max="10" width="10.625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="33.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="32.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -2654,7 +2854,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>14</v>
@@ -2676,10 +2876,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="32" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2687,7 +2887,7 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>10</v>
@@ -2698,23 +2898,23 @@
       <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="24" t="s">
-        <v>163</v>
+      <c r="I2" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>10</v>
@@ -2725,19 +2925,19 @@
       <c r="H3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="24"/>
+      <c r="I3" s="20"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>10</v>
@@ -2748,23 +2948,23 @@
       <c r="H4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="24" t="s">
-        <v>163</v>
+      <c r="I4" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="19" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>10</v>
@@ -2775,23 +2975,23 @@
       <c r="H5" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="24" t="s">
-        <v>163</v>
+      <c r="I5" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="7" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>10</v>
@@ -2802,23 +3002,23 @@
       <c r="H6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="24" t="s">
-        <v>163</v>
+      <c r="I6" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>10</v>
@@ -2829,23 +3029,23 @@
       <c r="H7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="24" t="s">
-        <v>163</v>
+      <c r="I7" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>81</v>
@@ -2856,21 +3056,21 @@
       <c r="H8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="24" t="s">
-        <v>163</v>
+      <c r="I8" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>45</v>
@@ -2879,25 +3079,25 @@
         <v>25</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>163</v>
+        <v>165</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>47</v>
@@ -2908,17 +3108,17 @@
       <c r="H10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="24"/>
+      <c r="I10" s="20"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>49</v>
@@ -2929,17 +3129,17 @@
       <c r="H11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="24"/>
+      <c r="I11" s="20"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
       <c r="E12" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>46</v>
@@ -2950,19 +3150,19 @@
       <c r="H12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="24"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>45</v>
@@ -2973,23 +3173,23 @@
       <c r="H13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="24" t="s">
-        <v>163</v>
+      <c r="I13" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>26</v>
@@ -3000,19 +3200,19 @@
       <c r="H14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="24"/>
+      <c r="I14" s="20"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>26</v>
@@ -3023,19 +3223,19 @@
       <c r="H15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="24"/>
+      <c r="I15" s="20"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23" t="s">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32" t="s">
         <v>40</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>51</v>
@@ -3046,17 +3246,17 @@
       <c r="H16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="24"/>
+      <c r="I16" s="20"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
       <c r="E17" s="6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>52</v>
@@ -3067,15 +3267,15 @@
       <c r="H17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="24"/>
+      <c r="I17" s="20"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="36" t="s">
         <v>87</v>
       </c>
       <c r="C18" s="10"/>
@@ -3083,7 +3283,7 @@
         <v>63</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>58</v>
@@ -3094,23 +3294,23 @@
       <c r="H18" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I18" s="24" t="s">
-        <v>163</v>
+      <c r="I18" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="29"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>60</v>
@@ -3121,23 +3321,23 @@
       <c r="H19" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I19" s="24" t="s">
-        <v>163</v>
+      <c r="I19" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="7" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="29"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="10"/>
       <c r="D20" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>60</v>
@@ -3148,23 +3348,23 @@
       <c r="H20" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I20" s="24" t="s">
-        <v>219</v>
+      <c r="I20" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="7" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="29"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="12"/>
       <c r="D21" s="11" t="s">
         <v>66</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>60</v>
@@ -3175,23 +3375,23 @@
       <c r="H21" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="I21" s="24" t="s">
-        <v>176</v>
+      <c r="I21" s="20" t="s">
+        <v>304</v>
       </c>
       <c r="J21" s="3"/>
-      <c r="K21" s="3" t="s">
-        <v>177</v>
+      <c r="K21" s="7" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="21"/>
-      <c r="B22" s="29"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="14"/>
-      <c r="D22" s="25" t="s">
-        <v>217</v>
+      <c r="D22" s="33" t="s">
+        <v>211</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>71</v>
@@ -3202,21 +3402,21 @@
       <c r="H22" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="I22" s="24" t="s">
-        <v>163</v>
+      <c r="I22" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="29"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="17"/>
-      <c r="D23" s="26"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="6" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>71</v>
@@ -3227,21 +3427,21 @@
       <c r="H23" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I23" s="24" t="s">
-        <v>219</v>
+      <c r="I23" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
-      <c r="B24" s="29"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="14"/>
-      <c r="D24" s="26"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>71</v>
@@ -3252,21 +3452,21 @@
       <c r="H24" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="I24" s="24" t="s">
-        <v>222</v>
+      <c r="I24" s="20" t="s">
+        <v>304</v>
       </c>
       <c r="J24" s="3"/>
-      <c r="K24" s="3" t="s">
-        <v>221</v>
+      <c r="K24" s="7" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
-      <c r="B25" s="29"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="26"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="6" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>71</v>
@@ -3277,19 +3477,19 @@
       <c r="H25" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="I25" s="24" t="s">
-        <v>219</v>
+      <c r="I25" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="21"/>
-      <c r="B26" s="29"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="16"/>
-      <c r="D26" s="26"/>
+      <c r="D26" s="34"/>
       <c r="E26" s="6" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>73</v>
@@ -3300,21 +3500,21 @@
       <c r="H26" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I26" s="24" t="s">
-        <v>222</v>
+      <c r="I26" s="20" t="s">
+        <v>304</v>
       </c>
       <c r="J26" s="3"/>
-      <c r="K26" s="3" t="s">
-        <v>221</v>
+      <c r="K26" s="7" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21"/>
-      <c r="B27" s="29"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="37"/>
       <c r="C27" s="18"/>
-      <c r="D27" s="26"/>
+      <c r="D27" s="34"/>
       <c r="E27" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>73</v>
@@ -3325,21 +3525,21 @@
       <c r="H27" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I27" s="24" t="s">
-        <v>219</v>
+      <c r="I27" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="21"/>
-      <c r="B28" s="29"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="16"/>
-      <c r="D28" s="26"/>
+      <c r="D28" s="34"/>
       <c r="E28" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>77</v>
@@ -3350,21 +3550,21 @@
       <c r="H28" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="I28" s="24" t="s">
-        <v>222</v>
+      <c r="I28" s="20" t="s">
+        <v>304</v>
       </c>
       <c r="J28" s="3"/>
-      <c r="K28" s="3" t="s">
-        <v>221</v>
+      <c r="K28" s="7" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="22"/>
-      <c r="B29" s="30"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="38"/>
       <c r="C29" s="13"/>
-      <c r="D29" s="27"/>
+      <c r="D29" s="35"/>
       <c r="E29" s="6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>88</v>
@@ -3375,25 +3575,25 @@
       <c r="H29" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I29" s="24" t="s">
-        <v>222</v>
+      <c r="I29" s="20" t="s">
+        <v>304</v>
       </c>
       <c r="J29" s="3"/>
-      <c r="K29" s="3" t="s">
-        <v>221</v>
+      <c r="K29" s="7" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="29" t="s">
         <v>93</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="39" t="s">
         <v>92</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="6" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>47</v>
@@ -3404,21 +3604,21 @@
       <c r="H30" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="I30" s="24" t="s">
-        <v>219</v>
+      <c r="I30" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="J30" s="3"/>
-      <c r="K30" s="3" t="s">
-        <v>271</v>
+      <c r="K30" s="7" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="21"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="3"/>
-      <c r="C31" s="21"/>
+      <c r="C31" s="30"/>
       <c r="D31" s="3"/>
       <c r="E31" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>47</v>
@@ -3429,21 +3629,21 @@
       <c r="H31" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I31" s="24" t="s">
-        <v>219</v>
+      <c r="I31" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="J31" s="3"/>
-      <c r="K31" s="3" t="s">
-        <v>271</v>
+      <c r="K31" s="7" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="21"/>
+      <c r="C32" s="30"/>
       <c r="D32" s="3"/>
       <c r="E32" s="6" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>99</v>
@@ -3454,21 +3654,21 @@
       <c r="H32" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="I32" s="24" t="s">
-        <v>219</v>
+      <c r="I32" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="J32" s="3"/>
-      <c r="K32" s="3" t="s">
-        <v>271</v>
+      <c r="K32" s="7" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="21"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="21"/>
+      <c r="C33" s="30"/>
       <c r="D33" s="3"/>
       <c r="E33" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>99</v>
@@ -3479,21 +3679,21 @@
       <c r="H33" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I33" s="24" t="s">
-        <v>219</v>
+      <c r="I33" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="J33" s="3"/>
-      <c r="K33" s="3" t="s">
-        <v>271</v>
+      <c r="K33" s="7" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="21"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="21"/>
+      <c r="C34" s="30"/>
       <c r="D34" s="3"/>
       <c r="E34" s="6" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>104</v>
@@ -3504,21 +3704,21 @@
       <c r="H34" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="I34" s="24" t="s">
-        <v>219</v>
+      <c r="I34" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="J34" s="3"/>
-      <c r="K34" s="3" t="s">
-        <v>271</v>
+      <c r="K34" s="7" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="3"/>
-      <c r="C35" s="22"/>
+      <c r="C35" s="31"/>
       <c r="D35" s="3"/>
       <c r="E35" s="6" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>104</v>
@@ -3529,25 +3729,25 @@
       <c r="H35" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="I35" s="24" t="s">
-        <v>163</v>
+      <c r="I35" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="J35" s="3"/>
-      <c r="K35" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A36" s="21"/>
+      <c r="K35" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="30"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>98</v>
@@ -3556,25 +3756,25 @@
         <v>109</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I36" s="24" t="s">
-        <v>163</v>
+        <v>310</v>
+      </c>
+      <c r="I36" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="J36" s="3"/>
-      <c r="K36" s="3" t="s">
-        <v>271</v>
+      <c r="K36" s="7" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="21"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>98</v>
@@ -3585,23 +3785,23 @@
       <c r="H37" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="I37" s="24" t="s">
-        <v>176</v>
+      <c r="I37" s="20" t="s">
+        <v>304</v>
       </c>
       <c r="J37" s="3"/>
-      <c r="K37" s="3" t="s">
-        <v>221</v>
+      <c r="K37" s="7" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A38" s="21"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>98</v>
@@ -3612,19 +3812,23 @@
       <c r="H38" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="I38" s="24"/>
+      <c r="I38" s="20" t="s">
+        <v>299</v>
+      </c>
       <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
+      <c r="K38" s="7" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="39" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A39" s="21"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>98</v>
@@ -3633,90 +3837,106 @@
         <v>112</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="I39" s="24"/>
+        <v>119</v>
+      </c>
+      <c r="I39" s="20" t="s">
+        <v>305</v>
+      </c>
       <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
+      <c r="K39" s="7" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="40" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A40" s="21"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>98</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="I40" s="24"/>
+        <v>309</v>
+      </c>
+      <c r="I40" s="20" t="s">
+        <v>299</v>
+      </c>
       <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
+      <c r="K40" s="7" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="41" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A41" s="21"/>
+      <c r="A41" s="30"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>98</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="I41" s="24"/>
+        <v>117</v>
+      </c>
+      <c r="I41" s="20" t="s">
+        <v>305</v>
+      </c>
       <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
+      <c r="K41" s="7" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="42" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="21"/>
+      <c r="A42" s="30"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>98</v>
       </c>
       <c r="G42" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H42" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H42" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="I42" s="24"/>
+      <c r="I42" s="20" t="s">
+        <v>305</v>
+      </c>
       <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-    </row>
-    <row r="43" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A43" s="21"/>
+      <c r="K42" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A43" s="30"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>99</v>
@@ -3725,21 +3945,25 @@
         <v>109</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I43" s="24"/>
+        <v>310</v>
+      </c>
+      <c r="I43" s="20" t="s">
+        <v>303</v>
+      </c>
       <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
+      <c r="K43" s="7" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="44" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="21"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>99</v>
@@ -3750,19 +3974,23 @@
       <c r="H44" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="I44" s="24"/>
+      <c r="I44" s="20" t="s">
+        <v>305</v>
+      </c>
       <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
+      <c r="K44" s="7" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="45" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A45" s="21"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>99</v>
@@ -3773,19 +4001,23 @@
       <c r="H45" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="I45" s="24"/>
+      <c r="I45" s="20" t="s">
+        <v>303</v>
+      </c>
       <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
+      <c r="K45" s="7" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="46" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A46" s="21"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>99</v>
@@ -3794,90 +4026,106 @@
         <v>112</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="I46" s="24"/>
+        <v>119</v>
+      </c>
+      <c r="I46" s="20" t="s">
+        <v>305</v>
+      </c>
       <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
+      <c r="K46" s="7" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="47" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A47" s="21"/>
+      <c r="A47" s="30"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>99</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="I47" s="24"/>
+        <v>309</v>
+      </c>
+      <c r="I47" s="20" t="s">
+        <v>303</v>
+      </c>
       <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
+      <c r="K47" s="7" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="48" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A48" s="21"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>99</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="I48" s="24"/>
+        <v>117</v>
+      </c>
+      <c r="I48" s="20" t="s">
+        <v>305</v>
+      </c>
       <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
+      <c r="K48" s="7" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="49" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="21"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>99</v>
       </c>
       <c r="G49" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H49" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H49" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="I49" s="24"/>
+      <c r="I49" s="20" t="s">
+        <v>305</v>
+      </c>
       <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-    </row>
-    <row r="50" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A50" s="21"/>
+      <c r="K49" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A50" s="30"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>104</v>
@@ -3886,21 +4134,25 @@
         <v>109</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I50" s="24"/>
+        <v>310</v>
+      </c>
+      <c r="I50" s="20" t="s">
+        <v>303</v>
+      </c>
       <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
+      <c r="K50" s="7" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="51" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A51" s="21"/>
+      <c r="A51" s="30"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>104</v>
@@ -3911,19 +4163,23 @@
       <c r="H51" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="I51" s="24"/>
+      <c r="I51" s="20" t="s">
+        <v>305</v>
+      </c>
       <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
+      <c r="K51" s="7" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="52" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A52" s="21"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>104</v>
@@ -3934,19 +4190,23 @@
       <c r="H52" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="I52" s="24"/>
+      <c r="I52" s="20" t="s">
+        <v>303</v>
+      </c>
       <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
+      <c r="K52" s="7" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="53" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A53" s="21"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>104</v>
@@ -3955,755 +4215,803 @@
         <v>112</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="I53" s="24"/>
+        <v>119</v>
+      </c>
+      <c r="I53" s="20" t="s">
+        <v>305</v>
+      </c>
       <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
+      <c r="K53" s="7" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="54" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A54" s="21"/>
+      <c r="A54" s="30"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>104</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="I54" s="24"/>
+        <v>309</v>
+      </c>
+      <c r="I54" s="20" t="s">
+        <v>303</v>
+      </c>
       <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
+      <c r="K54" s="7" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="55" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A55" s="21"/>
+      <c r="A55" s="30"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>104</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="I55" s="24"/>
+        <v>117</v>
+      </c>
+      <c r="I55" s="20" t="s">
+        <v>305</v>
+      </c>
       <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
+      <c r="K55" s="7" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="56" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A56" s="22"/>
+      <c r="A56" s="31"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>104</v>
       </c>
       <c r="G56" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H56" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H56" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="I56" s="24"/>
+      <c r="I56" s="20" t="s">
+        <v>305</v>
+      </c>
       <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
+      <c r="K56" s="7" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="57" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A57" s="20" t="s">
-        <v>226</v>
+      <c r="A57" s="29" t="s">
+        <v>217</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>98</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="I57" s="24"/>
+        <v>315</v>
+      </c>
+      <c r="I57" s="20" t="s">
+        <v>299</v>
+      </c>
       <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
+      <c r="K57" s="7" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="58" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A58" s="21"/>
+      <c r="A58" s="30"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>98</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="I58" s="24"/>
+        <v>316</v>
+      </c>
+      <c r="I58" s="20" t="s">
+        <v>299</v>
+      </c>
       <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
+      <c r="K58" s="7" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="59" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A59" s="21"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>99</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="I59" s="24"/>
+        <v>315</v>
+      </c>
+      <c r="I59" s="20" t="s">
+        <v>299</v>
+      </c>
       <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
+      <c r="K59" s="7" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="60" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A60" s="21"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>99</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="I60" s="24"/>
+        <v>316</v>
+      </c>
+      <c r="I60" s="20" t="s">
+        <v>299</v>
+      </c>
       <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
+      <c r="K60" s="7" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="61" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A61" s="21"/>
+      <c r="A61" s="30"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>104</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="I61" s="24"/>
+        <v>315</v>
+      </c>
+      <c r="I61" s="20" t="s">
+        <v>299</v>
+      </c>
       <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
+      <c r="K61" s="7" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="62" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A62" s="22"/>
+      <c r="A62" s="31"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>104</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="I62" s="24"/>
+        <v>316</v>
+      </c>
+      <c r="I62" s="20" t="s">
+        <v>299</v>
+      </c>
       <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
+      <c r="K62" s="7" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="63" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A63" s="20" t="s">
-        <v>227</v>
+      <c r="A63" s="29" t="s">
+        <v>218</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>229</v>
+        <v>216</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>313</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="I63" s="24"/>
+        <v>314</v>
+      </c>
+      <c r="I63" s="20" t="s">
+        <v>303</v>
+      </c>
       <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
+      <c r="K63" s="7" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="64" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A64" s="21"/>
+      <c r="A64" s="30"/>
       <c r="B64" s="19"/>
       <c r="C64" s="19"/>
-      <c r="D64" s="20" t="s">
-        <v>232</v>
+      <c r="D64" s="29" t="s">
+        <v>222</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="I64" s="24"/>
+        <v>241</v>
+      </c>
+      <c r="I64" s="20" t="s">
+        <v>299</v>
+      </c>
       <c r="J64" s="19"/>
-      <c r="K64" s="19"/>
+      <c r="K64" s="7" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="65" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A65" s="21"/>
+      <c r="A65" s="30"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
-      <c r="D65" s="21"/>
+      <c r="D65" s="30"/>
       <c r="E65" s="19" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="I65" s="24"/>
+        <v>220</v>
+      </c>
+      <c r="I65" s="20"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
     </row>
     <row r="66" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A66" s="21"/>
+      <c r="A66" s="30"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
-      <c r="D66" s="21"/>
+      <c r="D66" s="30"/>
       <c r="E66" s="19" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="I66" s="24"/>
+        <v>230</v>
+      </c>
+      <c r="I66" s="20"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
     </row>
     <row r="67" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A67" s="21"/>
+      <c r="A67" s="30"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
-      <c r="D67" s="21"/>
+      <c r="D67" s="30"/>
       <c r="E67" s="19" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="I67" s="24"/>
+        <v>225</v>
+      </c>
+      <c r="I67" s="20"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
     </row>
     <row r="68" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A68" s="21"/>
+      <c r="A68" s="30"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
-      <c r="D68" s="21"/>
+      <c r="D68" s="30"/>
       <c r="E68" s="19" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="I68" s="24"/>
+        <v>229</v>
+      </c>
+      <c r="I68" s="20"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
     </row>
     <row r="69" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A69" s="21"/>
+      <c r="A69" s="30"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
-      <c r="D69" s="21"/>
+      <c r="D69" s="30"/>
       <c r="E69" s="19" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="I69" s="24"/>
+        <v>232</v>
+      </c>
+      <c r="I69" s="20"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
     </row>
     <row r="70" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A70" s="21"/>
+      <c r="A70" s="30"/>
       <c r="B70" s="3"/>
       <c r="C70" s="7"/>
-      <c r="D70" s="21"/>
+      <c r="D70" s="30"/>
       <c r="E70" s="19" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="I70" s="24"/>
+        <v>230</v>
+      </c>
+      <c r="I70" s="20"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
     </row>
     <row r="71" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A71" s="21"/>
+      <c r="A71" s="30"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
-      <c r="D71" s="21"/>
+      <c r="D71" s="30"/>
       <c r="E71" s="19" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="I71" s="24"/>
+        <v>225</v>
+      </c>
+      <c r="I71" s="20"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
     </row>
     <row r="72" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A72" s="21"/>
+      <c r="A72" s="30"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
-      <c r="D72" s="22"/>
+      <c r="D72" s="31"/>
       <c r="E72" s="19" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="I72" s="24"/>
+        <v>229</v>
+      </c>
+      <c r="I72" s="20"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
     </row>
     <row r="73" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A73" s="21"/>
+      <c r="A73" s="30"/>
       <c r="B73" s="19"/>
       <c r="C73" s="19"/>
-      <c r="D73" s="20" t="s">
-        <v>244</v>
+      <c r="D73" s="29" t="s">
+        <v>234</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="I73" s="24"/>
+        <v>241</v>
+      </c>
+      <c r="I73" s="20"/>
       <c r="J73" s="19"/>
       <c r="K73" s="19"/>
     </row>
     <row r="74" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A74" s="21"/>
+      <c r="A74" s="30"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
-      <c r="D74" s="21"/>
+      <c r="D74" s="30"/>
       <c r="E74" s="19" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="F74" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="H74" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="G74" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="I74" s="24"/>
+      <c r="I74" s="20"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
     </row>
     <row r="75" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A75" s="21"/>
+      <c r="A75" s="30"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
-      <c r="D75" s="21"/>
+      <c r="D75" s="30"/>
       <c r="E75" s="19" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="F75" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="H75" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="G75" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="H75" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="I75" s="24"/>
+      <c r="I75" s="20"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
     </row>
     <row r="76" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A76" s="21"/>
+      <c r="A76" s="30"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
-      <c r="D76" s="21"/>
+      <c r="D76" s="30"/>
       <c r="E76" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="I76" s="24"/>
+        <v>239</v>
+      </c>
+      <c r="I76" s="20"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
     </row>
     <row r="77" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A77" s="21"/>
+      <c r="A77" s="30"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
-      <c r="D77" s="22"/>
+      <c r="D77" s="31"/>
       <c r="E77" s="19" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="I77" s="24"/>
+        <v>239</v>
+      </c>
+      <c r="I77" s="20"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
     </row>
     <row r="78" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A78" s="21"/>
+      <c r="A78" s="30"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
-      <c r="D78" s="20" t="s">
-        <v>253</v>
+      <c r="D78" s="29" t="s">
+        <v>243</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="I78" s="24"/>
+        <v>241</v>
+      </c>
+      <c r="I78" s="20"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
     </row>
     <row r="79" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A79" s="21"/>
+      <c r="A79" s="30"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
-      <c r="D79" s="21"/>
+      <c r="D79" s="30"/>
       <c r="E79" s="19" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="I79" s="24"/>
+        <v>246</v>
+      </c>
+      <c r="I79" s="20"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
     </row>
     <row r="80" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A80" s="21"/>
+      <c r="A80" s="30"/>
       <c r="B80" s="19"/>
       <c r="C80" s="19"/>
-      <c r="D80" s="21"/>
+      <c r="D80" s="30"/>
       <c r="E80" s="19" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="I80" s="24"/>
+        <v>248</v>
+      </c>
+      <c r="I80" s="20"/>
       <c r="J80" s="19"/>
       <c r="K80" s="19"/>
     </row>
     <row r="81" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A81" s="21"/>
+      <c r="A81" s="30"/>
       <c r="B81" s="19"/>
       <c r="C81" s="19"/>
-      <c r="D81" s="21"/>
+      <c r="D81" s="30"/>
       <c r="E81" s="19" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="I81" s="24"/>
+        <v>250</v>
+      </c>
+      <c r="I81" s="20"/>
       <c r="J81" s="19"/>
       <c r="K81" s="19"/>
     </row>
     <row r="82" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A82" s="21"/>
+      <c r="A82" s="30"/>
       <c r="B82" s="19"/>
       <c r="C82" s="19"/>
-      <c r="D82" s="21"/>
+      <c r="D82" s="30"/>
       <c r="E82" s="19" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="I82" s="24"/>
+        <v>249</v>
+      </c>
+      <c r="I82" s="20"/>
       <c r="J82" s="19"/>
       <c r="K82" s="19"/>
     </row>
     <row r="83" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A83" s="21"/>
+      <c r="A83" s="30"/>
       <c r="B83" s="19"/>
       <c r="C83" s="19"/>
-      <c r="D83" s="21"/>
+      <c r="D83" s="30"/>
       <c r="E83" s="19" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="G83" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H83" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="H83" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="I83" s="24"/>
+      <c r="I83" s="20"/>
       <c r="J83" s="19"/>
       <c r="K83" s="19"/>
     </row>
     <row r="84" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A84" s="21"/>
+      <c r="A84" s="30"/>
       <c r="B84" s="19"/>
       <c r="C84" s="19"/>
-      <c r="D84" s="21"/>
+      <c r="D84" s="30"/>
       <c r="E84" s="19" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="I84" s="24"/>
+        <v>249</v>
+      </c>
+      <c r="I84" s="20"/>
       <c r="J84" s="19"/>
       <c r="K84" s="19"/>
     </row>
     <row r="85" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A85" s="21"/>
+      <c r="A85" s="30"/>
       <c r="B85" s="19"/>
       <c r="C85" s="19"/>
-      <c r="D85" s="21"/>
+      <c r="D85" s="30"/>
       <c r="E85" s="19" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="I85" s="24"/>
+        <v>252</v>
+      </c>
+      <c r="I85" s="20"/>
       <c r="J85" s="19"/>
       <c r="K85" s="19"/>
     </row>
     <row r="86" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A86" s="22"/>
+      <c r="A86" s="31"/>
       <c r="B86" s="19"/>
       <c r="C86" s="19"/>
-      <c r="D86" s="22"/>
+      <c r="D86" s="31"/>
       <c r="E86" s="19" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="I86" s="24"/>
+        <v>254</v>
+      </c>
+      <c r="I86" s="20"/>
       <c r="J86" s="19"/>
       <c r="K86" s="19"/>
     </row>
     <row r="87" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A87" s="19" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B87" s="19"/>
       <c r="C87" s="19"/>
       <c r="D87" s="19"/>
       <c r="E87" s="19" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="I87" s="24"/>
+        <v>259</v>
+      </c>
+      <c r="I87" s="20"/>
       <c r="J87" s="19"/>
       <c r="K87" s="19"/>
     </row>
@@ -4729,8 +5037,11 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND(EXACT($I1, "NG"), LEN($I1)=2)</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(EXACT($I1, "NG"), LEN($I1)=2)</formula>
+      <formula>AND(EXACT($I1, "HLD"), LEN($I1)=3)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[update] 1. InitTest 수정 및 추가 2. SearchTest 수정 및 추가 3. package.json 수정 4. tc 수정
</commit_message>
<xml_diff>
--- a/TC Directory/To Do List Test Case.xlsx
+++ b/TC Directory/To Do List Test Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhsdb\Desktop\포트폴리오\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721D8355-61DA-4863-BE9B-8AB5664D46D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BA1829-870C-482D-B704-3110A775545D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6C457D58-EB79-43DF-AE70-B6D33573AE26}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="322">
   <si>
     <t>Depth1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -132,11 +132,6 @@
   </si>
   <si>
     <t>1. search bar 하단에 list 표시란 확인</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 사이트 접속
-2. list 존재</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -762,9 +757,6 @@
     <t>TC00000010</t>
   </si>
   <si>
-    <t>TC00000012</t>
-  </si>
-  <si>
     <t>TC00000013</t>
   </si>
   <si>
@@ -980,11 +972,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1. 기존의 "내용을 입력하세요." text 사라지며 입력한 text 표시
-2. 검색 결과 입력한 text와 제목이 일치하는 to do list 표시</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1. 생성한 to do 중 하나의 to do 제목을 search bar의 좌측 입력란에 입력
 2. 검색 버튼 클릭</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1102,11 +1089,6 @@
   <si>
     <t>1. 생성한 to do 중 하나의 to do 제목, 날짜를 search bar에 입력
 2. 검색 버튼 클릭</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 기존의 "내용을 입력하세요.", "연도-월-일" 에서 입력한 제목과 날짜로 변경되어 표시
-2. 검색 결과 입력한 제목, 날짜와 일치하는 to do list 표시</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1171,14 +1153,6 @@
   </si>
   <si>
     <t>자동화 테스트</t>
-  </si>
-  <si>
-    <t>자동화 테스트</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>자동화 테스트
-(빈값으로 확인)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1398,6 +1372,55 @@
     <t>1. alert 미표시
 자동화 테스트
 (20240217)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 입력한 text 표시
+2. 검색 결과 입력한 text와 제목이 일치하는 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동화 테스트
+(20240218)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>날짜 text 입력하는 방식으로 확인
+자동화 테스트
+(20240218)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 입력한 제목과 날짜 표시
+2. 검색 결과 입력한 제목, 날짜와 일치하는 to do list 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동화 테스트
+(20240219)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동화 테스트
+(20240208)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동화 테스트
+(20240208)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>빈값으로 확인
+자동화 테스트
+(20240208)</t>
+  </si>
+  <si>
+    <t>TC00000012</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1855,13 +1878,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1883,9 +1909,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2574,7 +2597,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -2720,41 +2743,41 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="O9" s="23" t="s">
         <v>291</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>289</v>
-      </c>
-      <c r="N9" s="22" t="s">
-        <v>296</v>
-      </c>
-      <c r="O9" s="23" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="N10" s="24" t="s">
         <v>292</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>290</v>
-      </c>
-      <c r="N10" s="24" t="s">
-        <v>298</v>
       </c>
       <c r="O10" s="25"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" s="24" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B12" s="21" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C12" s="26"/>
     </row>
@@ -2821,9 +2844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77A7E11-AD39-4C68-8EFB-0359E0A3990C}">
   <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2854,7 +2875,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>14</v>
@@ -2866,20 +2887,20 @@
         <v>8</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2887,7 +2908,7 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>10</v>
@@ -2899,22 +2920,22 @@
         <v>16</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J2" s="3"/>
-      <c r="K2" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32" t="s">
+      <c r="K2" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>10</v>
@@ -2925,19 +2946,23 @@
       <c r="H3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="20"/>
+      <c r="I3" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="K3" s="7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>10</v>
@@ -2949,22 +2974,22 @@
         <v>19</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J4" s="3"/>
-      <c r="K4" s="19" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
+      <c r="K4" s="7" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>10</v>
@@ -2973,25 +2998,25 @@
         <v>22</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>10</v>
@@ -3003,613 +3028,641 @@
         <v>20</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
+      <c r="K6" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="I7" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
-        <v>261</v>
+      <c r="K7" s="7" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32" t="s">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J8" s="3"/>
-      <c r="K8" s="3" t="s">
-        <v>261</v>
+      <c r="K8" s="7" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I9" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="6" t="s">
+      <c r="F13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="4" t="s">
+      <c r="F15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32" t="s">
+      <c r="G16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="I16" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="20"/>
+      <c r="I17" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="K17" s="7" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="18" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>87</v>
+      <c r="A18" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>86</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="H18" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A19" s="30"/>
-      <c r="B19" s="37"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="H19" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="7" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
-      <c r="B20" s="37"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="10"/>
       <c r="D20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I20" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="7" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A21" s="30"/>
-      <c r="B21" s="37"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="12"/>
       <c r="D21" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="H21" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I21" s="20" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="7" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A22" s="30"/>
-      <c r="B22" s="37"/>
+      <c r="B22" s="38"/>
       <c r="C22" s="14"/>
-      <c r="D22" s="33" t="s">
-        <v>211</v>
+      <c r="D22" s="34" t="s">
+        <v>209</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="30"/>
-      <c r="B23" s="37"/>
+      <c r="B23" s="38"/>
       <c r="C23" s="17"/>
-      <c r="D23" s="34"/>
+      <c r="D23" s="35"/>
       <c r="E23" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F23" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="H23" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I23" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="30"/>
-      <c r="B24" s="37"/>
+      <c r="B24" s="38"/>
       <c r="C24" s="14"/>
-      <c r="D24" s="34"/>
+      <c r="D24" s="35"/>
       <c r="E24" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="7" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30"/>
-      <c r="B25" s="37"/>
+      <c r="B25" s="38"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="34"/>
+      <c r="D25" s="35"/>
       <c r="E25" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I25" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="30"/>
-      <c r="B26" s="37"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="16"/>
-      <c r="D26" s="34"/>
+      <c r="D26" s="35"/>
       <c r="E26" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F26" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="I26" s="20" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="7" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="30"/>
-      <c r="B27" s="37"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="18"/>
-      <c r="D27" s="34"/>
+      <c r="D27" s="35"/>
       <c r="E27" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I27" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="30"/>
-      <c r="B28" s="37"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="16"/>
-      <c r="D28" s="34"/>
+      <c r="D28" s="35"/>
       <c r="E28" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I28" s="20" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="7" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="31"/>
-      <c r="B29" s="38"/>
+      <c r="B29" s="39"/>
       <c r="C29" s="13"/>
-      <c r="D29" s="35"/>
+      <c r="D29" s="36"/>
       <c r="E29" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F29" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="H29" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I29" s="20" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="7" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="29" t="s">
-        <v>93</v>
+      <c r="A30" s="32" t="s">
+        <v>92</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="39" t="s">
-        <v>92</v>
+      <c r="C30" s="29" t="s">
+        <v>91</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G30" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H30" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H30" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="I30" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="7" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -3618,23 +3671,23 @@
       <c r="C31" s="30"/>
       <c r="D31" s="3"/>
       <c r="E31" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G31" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H31" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H31" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="I31" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="7" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -3643,23 +3696,23 @@
       <c r="C32" s="30"/>
       <c r="D32" s="3"/>
       <c r="E32" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="H32" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="I32" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="7" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -3668,23 +3721,23 @@
       <c r="C33" s="30"/>
       <c r="D33" s="3"/>
       <c r="E33" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G33" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H33" s="5" t="s">
-        <v>103</v>
-      </c>
       <c r="I33" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J33" s="3"/>
       <c r="K33" s="7" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -3693,23 +3746,23 @@
       <c r="C34" s="30"/>
       <c r="D34" s="3"/>
       <c r="E34" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F34" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H34" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="I34" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="7" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -3718,52 +3771,52 @@
       <c r="C35" s="31"/>
       <c r="D35" s="3"/>
       <c r="E35" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G35" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H35" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="H35" s="5" t="s">
-        <v>108</v>
-      </c>
       <c r="I35" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="7" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A36" s="30"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="I36" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="7" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -3771,26 +3824,26 @@
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I37" s="20" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="7" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="66" x14ac:dyDescent="0.3">
@@ -3798,26 +3851,26 @@
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I38" s="20" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="J38" s="3"/>
       <c r="K38" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="66" x14ac:dyDescent="0.3">
@@ -3825,26 +3878,26 @@
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I39" s="20" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J39" s="3"/>
       <c r="K39" s="7" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="66" x14ac:dyDescent="0.3">
@@ -3852,26 +3905,26 @@
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="I40" s="20" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="J40" s="3"/>
       <c r="K40" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="66" x14ac:dyDescent="0.3">
@@ -3879,26 +3932,26 @@
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G41" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H41" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H41" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="I41" s="20" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="7" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -3906,26 +3959,26 @@
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I42" s="20" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J42" s="3"/>
       <c r="K42" s="7" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
@@ -3933,26 +3986,26 @@
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="I43" s="20" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="J43" s="3"/>
       <c r="K43" s="7" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -3960,26 +4013,26 @@
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I44" s="20" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J44" s="3"/>
       <c r="K44" s="7" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="66" x14ac:dyDescent="0.3">
@@ -3987,26 +4040,26 @@
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I45" s="20" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="7" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="66" x14ac:dyDescent="0.3">
@@ -4014,26 +4067,26 @@
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I46" s="20" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J46" s="3"/>
       <c r="K46" s="7" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="66" x14ac:dyDescent="0.3">
@@ -4041,26 +4094,26 @@
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="I47" s="20" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="7" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="66" x14ac:dyDescent="0.3">
@@ -4068,26 +4121,26 @@
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G48" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H48" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H48" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="I48" s="20" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="7" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -4095,26 +4148,26 @@
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I49" s="20" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J49" s="3"/>
       <c r="K49" s="7" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
@@ -4122,26 +4175,26 @@
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="I50" s="20" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="7" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -4149,26 +4202,26 @@
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I51" s="20" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J51" s="3"/>
       <c r="K51" s="7" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="66" x14ac:dyDescent="0.3">
@@ -4176,26 +4229,26 @@
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I52" s="20" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="J52" s="3"/>
       <c r="K52" s="7" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="66" x14ac:dyDescent="0.3">
@@ -4203,26 +4256,26 @@
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I53" s="20" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J53" s="3"/>
       <c r="K53" s="7" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="66" x14ac:dyDescent="0.3">
@@ -4230,26 +4283,26 @@
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="I54" s="20" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="J54" s="3"/>
       <c r="K54" s="7" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="66" x14ac:dyDescent="0.3">
@@ -4257,26 +4310,26 @@
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G55" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H55" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H55" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="I55" s="20" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J55" s="3"/>
       <c r="K55" s="7" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -4284,55 +4337,55 @@
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I56" s="20" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J56" s="3"/>
       <c r="K56" s="7" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A57" s="29" t="s">
-        <v>217</v>
+      <c r="A57" s="32" t="s">
+        <v>215</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="I57" s="20" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="J57" s="3"/>
       <c r="K57" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -4340,26 +4393,26 @@
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="I58" s="20" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="J58" s="3"/>
       <c r="K58" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -4367,26 +4420,26 @@
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="I59" s="20" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="J59" s="3"/>
       <c r="K59" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -4394,26 +4447,26 @@
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="I60" s="20" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="J60" s="3"/>
       <c r="K60" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -4421,26 +4474,26 @@
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="I61" s="20" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="J61" s="3"/>
       <c r="K61" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -4448,82 +4501,82 @@
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="I62" s="20" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="J62" s="3"/>
       <c r="K62" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A63" s="29" t="s">
-        <v>218</v>
+      <c r="A63" s="32" t="s">
+        <v>216</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="I63" s="20" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="J63" s="3"/>
       <c r="K63" s="7" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A64" s="30"/>
       <c r="B64" s="19"/>
       <c r="C64" s="19"/>
-      <c r="D64" s="29" t="s">
-        <v>222</v>
+      <c r="D64" s="32" t="s">
+        <v>219</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I64" s="20" t="s">
-        <v>299</v>
+        <v>157</v>
       </c>
       <c r="J64" s="19"/>
       <c r="K64" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="66" x14ac:dyDescent="0.3">
@@ -4532,20 +4585,24 @@
       <c r="C65" s="3"/>
       <c r="D65" s="30"/>
       <c r="E65" s="19" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="I65" s="20"/>
+        <v>312</v>
+      </c>
+      <c r="I65" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J65" s="3"/>
-      <c r="K65" s="3"/>
+      <c r="K65" s="7" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="66" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A66" s="30"/>
@@ -4553,20 +4610,24 @@
       <c r="C66" s="3"/>
       <c r="D66" s="30"/>
       <c r="E66" s="19" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="I66" s="20"/>
+        <v>227</v>
+      </c>
+      <c r="I66" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J66" s="3"/>
-      <c r="K66" s="3"/>
+      <c r="K66" s="7" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="67" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A67" s="30"/>
@@ -4574,20 +4635,24 @@
       <c r="C67" s="3"/>
       <c r="D67" s="30"/>
       <c r="E67" s="19" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="I67" s="20"/>
+        <v>222</v>
+      </c>
+      <c r="I67" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
+      <c r="K67" s="7" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="68" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A68" s="30"/>
@@ -4595,20 +4660,24 @@
       <c r="C68" s="3"/>
       <c r="D68" s="30"/>
       <c r="E68" s="19" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="I68" s="20"/>
+        <v>226</v>
+      </c>
+      <c r="I68" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
+      <c r="K68" s="7" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="69" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A69" s="30"/>
@@ -4616,20 +4685,24 @@
       <c r="C69" s="3"/>
       <c r="D69" s="30"/>
       <c r="E69" s="19" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="I69" s="20"/>
+        <v>229</v>
+      </c>
+      <c r="I69" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J69" s="3"/>
-      <c r="K69" s="3"/>
+      <c r="K69" s="7" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="70" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A70" s="30"/>
@@ -4637,20 +4710,24 @@
       <c r="C70" s="7"/>
       <c r="D70" s="30"/>
       <c r="E70" s="19" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="I70" s="20"/>
+        <v>227</v>
+      </c>
+      <c r="I70" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J70" s="3"/>
-      <c r="K70" s="3"/>
+      <c r="K70" s="7" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="71" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A71" s="30"/>
@@ -4658,20 +4735,24 @@
       <c r="C71" s="3"/>
       <c r="D71" s="30"/>
       <c r="E71" s="19" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="I71" s="20"/>
+        <v>222</v>
+      </c>
+      <c r="I71" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J71" s="3"/>
-      <c r="K71" s="3"/>
+      <c r="K71" s="7" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="72" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A72" s="30"/>
@@ -4679,43 +4760,51 @@
       <c r="C72" s="3"/>
       <c r="D72" s="31"/>
       <c r="E72" s="19" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="I72" s="20"/>
+        <v>226</v>
+      </c>
+      <c r="I72" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J72" s="3"/>
-      <c r="K72" s="3"/>
+      <c r="K72" s="7" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="73" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A73" s="30"/>
       <c r="B73" s="19"/>
       <c r="C73" s="19"/>
-      <c r="D73" s="29" t="s">
-        <v>234</v>
+      <c r="D73" s="32" t="s">
+        <v>231</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="I73" s="20"/>
+        <v>238</v>
+      </c>
+      <c r="I73" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J73" s="19"/>
-      <c r="K73" s="19"/>
+      <c r="K73" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="74" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A74" s="30"/>
@@ -4723,20 +4812,24 @@
       <c r="C74" s="3"/>
       <c r="D74" s="30"/>
       <c r="E74" s="19" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="I74" s="20"/>
+        <v>233</v>
+      </c>
+      <c r="I74" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
+      <c r="K74" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="75" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A75" s="30"/>
@@ -4744,20 +4837,24 @@
       <c r="C75" s="3"/>
       <c r="D75" s="30"/>
       <c r="E75" s="19" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="I75" s="20"/>
+        <v>234</v>
+      </c>
+      <c r="I75" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J75" s="3"/>
-      <c r="K75" s="3"/>
+      <c r="K75" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="76" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A76" s="30"/>
@@ -4765,20 +4862,24 @@
       <c r="C76" s="3"/>
       <c r="D76" s="30"/>
       <c r="E76" s="19" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="I76" s="20"/>
+        <v>236</v>
+      </c>
+      <c r="I76" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J76" s="3"/>
-      <c r="K76" s="3"/>
+      <c r="K76" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="77" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A77" s="30"/>
@@ -4786,43 +4887,51 @@
       <c r="C77" s="3"/>
       <c r="D77" s="31"/>
       <c r="E77" s="19" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="I77" s="20"/>
+        <v>236</v>
+      </c>
+      <c r="I77" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
+      <c r="K77" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="78" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A78" s="30"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
-      <c r="D78" s="29" t="s">
-        <v>243</v>
+      <c r="D78" s="32" t="s">
+        <v>240</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="I78" s="20"/>
+        <v>238</v>
+      </c>
+      <c r="I78" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J78" s="3"/>
-      <c r="K78" s="3"/>
+      <c r="K78" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="79" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A79" s="30"/>
@@ -4830,20 +4939,24 @@
       <c r="C79" s="3"/>
       <c r="D79" s="30"/>
       <c r="E79" s="19" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="I79" s="20"/>
+        <v>316</v>
+      </c>
+      <c r="I79" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J79" s="3"/>
-      <c r="K79" s="3"/>
+      <c r="K79" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="80" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A80" s="30"/>
@@ -4851,20 +4964,24 @@
       <c r="C80" s="19"/>
       <c r="D80" s="30"/>
       <c r="E80" s="19" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="I80" s="20"/>
+        <v>244</v>
+      </c>
+      <c r="I80" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J80" s="19"/>
-      <c r="K80" s="19"/>
+      <c r="K80" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="81" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A81" s="30"/>
@@ -4872,20 +4989,24 @@
       <c r="C81" s="19"/>
       <c r="D81" s="30"/>
       <c r="E81" s="19" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="I81" s="20"/>
+        <v>246</v>
+      </c>
+      <c r="I81" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J81" s="19"/>
-      <c r="K81" s="19"/>
+      <c r="K81" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="82" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A82" s="30"/>
@@ -4893,20 +5014,24 @@
       <c r="C82" s="19"/>
       <c r="D82" s="30"/>
       <c r="E82" s="19" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="I82" s="20"/>
+        <v>245</v>
+      </c>
+      <c r="I82" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J82" s="19"/>
-      <c r="K82" s="19"/>
+      <c r="K82" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="83" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A83" s="30"/>
@@ -4914,20 +5039,24 @@
       <c r="C83" s="19"/>
       <c r="D83" s="30"/>
       <c r="E83" s="19" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="I83" s="20"/>
+        <v>251</v>
+      </c>
+      <c r="I83" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J83" s="19"/>
-      <c r="K83" s="19"/>
+      <c r="K83" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="84" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A84" s="30"/>
@@ -4935,20 +5064,24 @@
       <c r="C84" s="19"/>
       <c r="D84" s="30"/>
       <c r="E84" s="19" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="I84" s="20"/>
+        <v>245</v>
+      </c>
+      <c r="I84" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J84" s="19"/>
-      <c r="K84" s="19"/>
+      <c r="K84" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="85" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A85" s="30"/>
@@ -4956,20 +5089,24 @@
       <c r="C85" s="19"/>
       <c r="D85" s="30"/>
       <c r="E85" s="19" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="I85" s="20"/>
+        <v>248</v>
+      </c>
+      <c r="I85" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J85" s="19"/>
-      <c r="K85" s="19"/>
+      <c r="K85" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="86" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A86" s="31"/>
@@ -4977,54 +5114,55 @@
       <c r="C86" s="19"/>
       <c r="D86" s="31"/>
       <c r="E86" s="19" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="I86" s="20"/>
+        <v>250</v>
+      </c>
+      <c r="I86" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J86" s="19"/>
-      <c r="K86" s="19"/>
+      <c r="K86" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="87" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A87" s="19" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B87" s="19"/>
       <c r="C87" s="19"/>
       <c r="D87" s="19"/>
       <c r="E87" s="19" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="I87" s="20"/>
+        <v>255</v>
+      </c>
+      <c r="I87" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="J87" s="19"/>
-      <c r="K87" s="19"/>
+      <c r="K87" s="7" t="s">
+        <v>317</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K87" xr:uid="{E77A7E11-AD39-4C68-8EFB-0359E0A3990C}"/>
   <mergeCells count="16">
-    <mergeCell ref="C30:C35"/>
-    <mergeCell ref="A30:A56"/>
-    <mergeCell ref="A57:A62"/>
-    <mergeCell ref="A63:A86"/>
-    <mergeCell ref="D64:D72"/>
-    <mergeCell ref="D73:D77"/>
-    <mergeCell ref="D78:D86"/>
     <mergeCell ref="A18:A29"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="C8:C17"/>
@@ -5034,6 +5172,13 @@
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="D22:D29"/>
     <mergeCell ref="B18:B29"/>
+    <mergeCell ref="C30:C35"/>
+    <mergeCell ref="A30:A56"/>
+    <mergeCell ref="A57:A62"/>
+    <mergeCell ref="A63:A86"/>
+    <mergeCell ref="D64:D72"/>
+    <mergeCell ref="D73:D77"/>
+    <mergeCell ref="D78:D86"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1:I1048576">

</xml_diff>